<commit_message>
updated add to basket
</commit_message>
<xml_diff>
--- a/src/test/resources/TESTDATA.xlsx
+++ b/src/test/resources/TESTDATA.xlsx
@@ -3,20 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100800_{A77C109E-6D77-42DD-B8B0-0924CE67ACA7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace3\SDET34L1PracticeTestCases\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5718D6E1-A65A-4698-B996-69D5D51584DA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3015" activeTab="2" xr2:uid="{E0DC2931-42F9-46E3-B13D-FE28EAFC11AD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11430" windowHeight="3015" activeTab="1" xr2:uid="{E0DC2931-42F9-46E3-B13D-FE28EAFC11AD}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="documents" sheetId="5" r:id="rId2"/>
-    <sheet name="organization" sheetId="4" r:id="rId3"/>
-    <sheet name="logindata" sheetId="3" r:id="rId4"/>
-    <sheet name="campaign" sheetId="2" r:id="rId5"/>
-    <sheet name="products" sheetId="6" r:id="rId6"/>
+    <sheet name="checkout" sheetId="7" r:id="rId2"/>
+    <sheet name="documents" sheetId="5" r:id="rId3"/>
+    <sheet name="organization" sheetId="4" r:id="rId4"/>
+    <sheet name="logindata" sheetId="3" r:id="rId5"/>
+    <sheet name="campaign" sheetId="2" r:id="rId6"/>
+    <sheet name="products" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>TestCase</t>
   </si>
@@ -315,6 +320,15 @@
   </si>
   <si>
     <t>pwd</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>Sanjay</t>
+  </si>
+  <si>
+    <t>Billing Details</t>
   </si>
 </sst>
 </file>
@@ -874,6 +888,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4433E54F-0080-4620-9EE8-EDCE94AE4626}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946C5BF3-C7A5-4A36-AB6A-5804F393F38A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -931,11 +973,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0A9AFA-FBE2-4DE0-AC84-FC34353EEC18}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1010,7 +1052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA37E02-312E-4FB9-9E85-4D3AEE0FEF31}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1193,7 +1235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018E61FD-CEE0-4EA7-BDF4-DA3CB4EDDA7D}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1259,7 +1301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EDFA70-DAD7-457F-8BBD-CA6A56E92FE6}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>